<commit_message>
reorganização do notebook - seções e subseções - seção de resultado criada - falta tabela e relatório com IA
</commit_message>
<xml_diff>
--- a/0.96 - ALPHA - Teste Global/dados_contabeis_global.xlsx
+++ b/0.96 - ALPHA - Teste Global/dados_contabeis_global.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/Desktop OneDrive/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/5. Trabalho/1. Expediente/1. Ativos/a. Economia/CONSULTORIAS/Metodo Score Assertif Pay/Github/FinScore/0.96 - ALPHA - Teste Global/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{71EC5D9A-557B-41A7-A6BB-40BBD76DF2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E41FD0F-2B95-438F-99DF-1F4FA1675ED4}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{71EC5D9A-557B-41A7-A6BB-40BBD76DF2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F429A33-3022-4553-B05C-40303709A03D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -476,7 +476,7 @@
     <col min="3" max="3" width="27.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.21875" style="1" customWidth="1"/>
     <col min="8" max="8" width="28.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.88671875" style="1" bestFit="1" customWidth="1"/>

</xml_diff>